<commit_message>
code of the task and updated excel file
</commit_message>
<xml_diff>
--- a/taskupdates.xlsx
+++ b/taskupdates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dharmik\Internship\project-phase2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42F97DF5-545E-4254-8AF1-5503961C5B1E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EFED3D-7748-4B29-B8F9-CFD6E2D5715C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{17C284EA-58CC-46CB-BC8B-1AA8C0E68204}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -34,6 +34,24 @@
   </si>
   <si>
     <t>Made a GIT repository</t>
+  </si>
+  <si>
+    <t>no updates</t>
+  </si>
+  <si>
+    <t>Eclipse setup</t>
+  </si>
+  <si>
+    <t>meeting on task updates</t>
+  </si>
+  <si>
+    <t>java and spring basics</t>
+  </si>
+  <si>
+    <t>started the task</t>
+  </si>
+  <si>
+    <t>continued the task</t>
   </si>
 </sst>
 </file>
@@ -386,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C766E0-AB49-470E-993F-36C56B99A79E}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,6 +432,62 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43492</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43493</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43494</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43495</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43496</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43497</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43498</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>